<commit_message>
[update] update total apf area
</commit_message>
<xml_diff>
--- a/simulation/python/Book1.xlsx
+++ b/simulation/python/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APF\junbot_adaptive_planner\simulation\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5BDF17-F1E7-4277-B871-55C536EFA041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85B93C-3CAC-4A52-8A4A-6D6E48782296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,9 +372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -383,16 +385,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B1">
         <v>250</v>
       </c>
       <c r="C1">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D1">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -430,6 +432,74 @@
       </c>
       <c r="E3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>350</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>300</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>